<commit_message>
[UPDATE] Implement verbosity config.
</commit_message>
<xml_diff>
--- a/examples/regression/skl_regressor_test_summary.xlsx
+++ b/examples/regression/skl_regressor_test_summary.xlsx
@@ -497,36 +497,36 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>default</t>
+          <t>n_estimators: 50/loss: exponential/learning_rate: 0.3</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.998880691478474</v>
+        <v>0.9968105280705966</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9985075886379654</v>
+        <v>0.9957473707607954</v>
       </c>
       <c r="F2" t="n">
-        <v>3.482987899999994</v>
+        <v>6.109256117647064</v>
       </c>
       <c r="G2" t="n">
-        <v>1.68404716715686</v>
+        <v>2.488673687089965</v>
       </c>
       <c r="H2" t="n">
-        <v>1.297708429176932</v>
+        <v>1.577553069500347</v>
       </c>
       <c r="I2" t="n">
-        <v>3.846727533034194</v>
+        <v>8.364261831033858</v>
       </c>
       <c r="J2" t="n">
-        <v>1.961307607958067</v>
+        <v>2.892103357598732</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1211500883024353</v>
+        <v>0.2155627060651892</v>
       </c>
     </row>
     <row r="3">
@@ -536,36 +536,36 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>n_estimators: 500/max_samples: 1.0</t>
+          <t>n_estimators: 100/max_samples: 1.0</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.9992383176962081</v>
+        <v>0.9988560555848621</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9989844235949441</v>
+        <v>0.9984747407798161</v>
       </c>
       <c r="F3" t="n">
-        <v>3.272173561999672</v>
+        <v>3.425956200000073</v>
       </c>
       <c r="G3" t="n">
-        <v>1.246881543529481</v>
+        <v>1.322533833529427</v>
       </c>
       <c r="H3" t="n">
-        <v>1.116638501722684</v>
+        <v>1.150014710136104</v>
       </c>
       <c r="I3" t="n">
-        <v>2.283280912636512</v>
+        <v>2.999948210910336</v>
       </c>
       <c r="J3" t="n">
-        <v>1.511052915233782</v>
+        <v>1.732035857281926</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1429446367864206</v>
+        <v>0.1316424817931592</v>
       </c>
     </row>
     <row r="4">
@@ -575,36 +575,36 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>normalize: False/n_iter: 300/lambda_2: 10/lambda_1: 1/fit_intercept: True/copy_X: True/compute_score: True/alpha_2: 100/alpha_1: 0.001</t>
+          <t>default</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.9911258055386907</v>
+        <v>0.9862461086791027</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9881677407182542</v>
+        <v>0.9816614782388036</v>
       </c>
       <c r="F4" t="n">
-        <v>9.664265530081465</v>
+        <v>9.578972520548049</v>
       </c>
       <c r="G4" t="n">
-        <v>4.346491140253007</v>
+        <v>5.554871476977115</v>
       </c>
       <c r="H4" t="n">
-        <v>2.084824007021457</v>
+        <v>2.356877484507227</v>
       </c>
       <c r="I4" t="n">
-        <v>26.62798664777845</v>
+        <v>36.06902670721665</v>
       </c>
       <c r="J4" t="n">
-        <v>5.160231259137371</v>
+        <v>6.005749470900085</v>
       </c>
       <c r="K4" t="n">
-        <v>1.004752962128791</v>
+        <v>0.4012172529941787</v>
       </c>
     </row>
     <row r="5">
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -622,28 +622,28 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.99888092919921</v>
+        <v>0.9979738033433034</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9985079055989466</v>
+        <v>0.9972984044577379</v>
       </c>
       <c r="F5" t="n">
-        <v>4.509007000000004</v>
+        <v>4.138573999999991</v>
       </c>
       <c r="G5" t="n">
-        <v>1.264202</v>
+        <v>1.993801235294116</v>
       </c>
       <c r="H5" t="n">
-        <v>1.124367377684002</v>
+        <v>1.412020267309969</v>
       </c>
       <c r="I5" t="n">
-        <v>3.354617780421175</v>
+        <v>5.313619223777232</v>
       </c>
       <c r="J5" t="n">
-        <v>1.831561568831683</v>
+        <v>2.305128895263176</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1170784342525696</v>
+        <v>0.1371398890472471</v>
       </c>
     </row>
     <row r="6">
@@ -653,7 +653,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -661,28 +661,28 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>-0.003783948064497222</v>
+        <v>-5.856187952280045e-05</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.3383785974193296</v>
+        <v>-0.3334114158393637</v>
       </c>
       <c r="F6" t="n">
-        <v>81.92140995312499</v>
+        <v>79.26752778125</v>
       </c>
       <c r="G6" t="n">
-        <v>36.61843377297794</v>
+        <v>41.21908382904412</v>
       </c>
       <c r="H6" t="n">
-        <v>6.051316697461631</v>
+        <v>6.420209017551073</v>
       </c>
       <c r="I6" t="n">
-        <v>2168.608352328596</v>
+        <v>2510.325650115235</v>
       </c>
       <c r="J6" t="n">
-        <v>46.56831919157697</v>
+        <v>50.10315010171751</v>
       </c>
       <c r="K6" t="n">
-        <v>2.299945243503828</v>
+        <v>3.827869832326928</v>
       </c>
     </row>
     <row r="7">
@@ -692,36 +692,36 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>normalize: False/l1_ratio: 1/fit_intercept: True/alpha: 0.05</t>
+          <t>normalize: False/l1_ratio: 0.75/fit_intercept: False/alpha: 0.02</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.9911679500893532</v>
+        <v>0.9542793937512544</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9882239334524709</v>
+        <v>0.9390391916683392</v>
       </c>
       <c r="F7" t="n">
-        <v>9.747981167211847</v>
+        <v>19.20629528732702</v>
       </c>
       <c r="G7" t="n">
-        <v>4.338207834004342</v>
+        <v>9.006199801404126</v>
       </c>
       <c r="H7" t="n">
-        <v>2.082836487582341</v>
+        <v>3.001033122343725</v>
       </c>
       <c r="I7" t="n">
-        <v>26.50152733508125</v>
+        <v>119.9004506710438</v>
       </c>
       <c r="J7" t="n">
-        <v>5.147963416253194</v>
+        <v>10.94990642293549</v>
       </c>
       <c r="K7" t="n">
-        <v>0.9853653430173551</v>
+        <v>0.5675978780939747</v>
       </c>
     </row>
     <row r="8">
@@ -731,36 +731,36 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>normalize: False/l1_ratio: 0.75/fit_intercept: True</t>
+          <t>default</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.9913240437352692</v>
+        <v>0.9842965028627755</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9884320583136922</v>
+        <v>0.979062003817034</v>
       </c>
       <c r="F8" t="n">
-        <v>8.552720422978879</v>
+        <v>9.819193363552763</v>
       </c>
       <c r="G8" t="n">
-        <v>4.547692358369694</v>
+        <v>5.825573130736727</v>
       </c>
       <c r="H8" t="n">
-        <v>2.132531912626325</v>
+        <v>2.413622408484129</v>
       </c>
       <c r="I8" t="n">
-        <v>26.03315135601368</v>
+        <v>39.41858323376366</v>
       </c>
       <c r="J8" t="n">
-        <v>5.102269235939406</v>
+        <v>6.278422033740934</v>
       </c>
       <c r="K8" t="n">
-        <v>0.9430811145279925</v>
+        <v>2.555655046335292</v>
       </c>
     </row>
     <row r="9">
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -778,28 +778,28 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.9983565279495907</v>
+        <v>0.9986523022906715</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9978087039327876</v>
+        <v>0.9982030697208953</v>
       </c>
       <c r="F9" t="n">
         <v>4.138573999999991</v>
       </c>
       <c r="G9" t="n">
-        <v>1.516268</v>
+        <v>1.411778411764706</v>
       </c>
       <c r="H9" t="n">
-        <v>1.23136834456632</v>
+        <v>1.188182819167449</v>
       </c>
       <c r="I9" t="n">
-        <v>3.550611884368466</v>
+        <v>3.534283028481468</v>
       </c>
       <c r="J9" t="n">
-        <v>1.884306738397034</v>
+        <v>1.879968890296185</v>
       </c>
       <c r="K9" t="n">
-        <v>0.175722574099342</v>
+        <v>0.04215737014596937</v>
       </c>
     </row>
     <row r="10">
@@ -809,7 +809,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -817,28 +817,28 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.9995073371156706</v>
+        <v>0.9992304978263927</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9993431161542276</v>
+        <v>0.998973997101857</v>
       </c>
       <c r="F10" t="n">
-        <v>3.067083729999958</v>
+        <v>2.795443600000084</v>
       </c>
       <c r="G10" t="n">
-        <v>0.8109707376470584</v>
+        <v>1.158941678823537</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9005391372100706</v>
+        <v>1.076541536041939</v>
       </c>
       <c r="I10" t="n">
-        <v>1.476846389306288</v>
+        <v>2.017988495294463</v>
       </c>
       <c r="J10" t="n">
-        <v>1.215255688859874</v>
+        <v>1.420559219214202</v>
       </c>
       <c r="K10" t="n">
-        <v>0.1272090329239975</v>
+        <v>0.06739951589098545</v>
       </c>
     </row>
     <row r="11">
@@ -848,7 +848,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -856,28 +856,28 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.9991561211304549</v>
+        <v>0.9989388349822468</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9988748281739399</v>
+        <v>0.9985851133096624</v>
       </c>
       <c r="F11" t="n">
-        <v>4.09211224793944</v>
+        <v>5.394667161180289</v>
       </c>
       <c r="G11" t="n">
-        <v>1.096665431815591</v>
+        <v>1.132850583870979</v>
       </c>
       <c r="H11" t="n">
-        <v>1.047217948574026</v>
+        <v>1.064354538615296</v>
       </c>
       <c r="I11" t="n">
-        <v>2.52968003302325</v>
+        <v>2.782862571260226</v>
       </c>
       <c r="J11" t="n">
-        <v>1.59049678812101</v>
+        <v>1.668191407261237</v>
       </c>
       <c r="K11" t="n">
-        <v>0.1239021401765846</v>
+        <v>0.2001410298244644</v>
       </c>
     </row>
     <row r="12">
@@ -887,7 +887,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -895,28 +895,28 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.9911374860652171</v>
+        <v>0.9855508370577364</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9881833147536229</v>
+        <v>0.9807344494103152</v>
       </c>
       <c r="F12" t="n">
-        <v>9.966100881860299</v>
+        <v>10.80352007121122</v>
       </c>
       <c r="G12" t="n">
-        <v>4.303183486642582</v>
+        <v>5.440576472896923</v>
       </c>
       <c r="H12" t="n">
-        <v>2.074411600103167</v>
+        <v>2.332504335022108</v>
       </c>
       <c r="I12" t="n">
-        <v>26.59293795623364</v>
+        <v>36.26998031844126</v>
       </c>
       <c r="J12" t="n">
-        <v>5.156834102066271</v>
+        <v>6.022456335951408</v>
       </c>
       <c r="K12" t="n">
-        <v>0.9834048444621972</v>
+        <v>2.759056682813132</v>
       </c>
     </row>
     <row r="13">
@@ -926,36 +926,36 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>weights: distance/n_neighbors: 5/metric: euclidean/algorithm: brute</t>
+          <t>default</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.9470845839983579</v>
+        <v>0.9337517906779914</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9294461119978106</v>
+        <v>0.9116690542373219</v>
       </c>
       <c r="F13" t="n">
-        <v>21.15983404374725</v>
+        <v>27.6298188</v>
       </c>
       <c r="G13" t="n">
-        <v>8.074651711930015</v>
+        <v>10.96940407058823</v>
       </c>
       <c r="H13" t="n">
-        <v>2.841593164393878</v>
+        <v>3.312009068615036</v>
       </c>
       <c r="I13" t="n">
-        <v>114.3202312901799</v>
+        <v>173.7332639607421</v>
       </c>
       <c r="J13" t="n">
-        <v>10.69206393967881</v>
+        <v>13.18079147702224</v>
       </c>
       <c r="K13" t="n">
-        <v>0.6918292418767168</v>
+        <v>0.870974381660599</v>
       </c>
     </row>
     <row r="14">
@@ -965,7 +965,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -973,28 +973,28 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.9910718957713713</v>
+        <v>0.9862975178373595</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9880958610284951</v>
+        <v>0.981730023783146</v>
       </c>
       <c r="F14" t="n">
-        <v>9.759519116259199</v>
+        <v>9.527663346272767</v>
       </c>
       <c r="G14" t="n">
-        <v>4.342011314858294</v>
+        <v>5.547959643245941</v>
       </c>
       <c r="H14" t="n">
-        <v>2.083749340697747</v>
+        <v>2.35541071646665</v>
       </c>
       <c r="I14" t="n">
-        <v>26.78974877397739</v>
+        <v>35.93420825773965</v>
       </c>
       <c r="J14" t="n">
-        <v>5.17588144898793</v>
+        <v>5.994514847570206</v>
       </c>
       <c r="K14" t="n">
-        <v>1.008249996397359</v>
+        <v>0.4012007676083679</v>
       </c>
     </row>
     <row r="15">
@@ -1004,7 +1004,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1012,28 +1012,28 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.9913080623967049</v>
+        <v>0.9859272148331321</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9884107498622732</v>
+        <v>0.981236286444176</v>
       </c>
       <c r="F15" t="n">
-        <v>9.730655344942974</v>
+        <v>10.82754213475699</v>
       </c>
       <c r="G15" t="n">
-        <v>4.327341162846548</v>
+        <v>5.419625058810348</v>
       </c>
       <c r="H15" t="n">
-        <v>2.080226228766128</v>
+        <v>2.328008818456311</v>
       </c>
       <c r="I15" t="n">
-        <v>26.08110510232365</v>
+        <v>35.3252048625585</v>
       </c>
       <c r="J15" t="n">
-        <v>5.106966330643237</v>
+        <v>5.943501061037888</v>
       </c>
       <c r="K15" t="n">
-        <v>0.9478701580016372</v>
+        <v>2.477894955344792</v>
       </c>
     </row>
     <row r="16">
@@ -1043,7 +1043,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1051,28 +1051,28 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.9901399074703277</v>
+        <v>0.9863099920604954</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9868532099604369</v>
+        <v>0.9817466560806606</v>
       </c>
       <c r="F16" t="n">
-        <v>9.494716471818421</v>
+        <v>10.82413047261112</v>
       </c>
       <c r="G16" t="n">
-        <v>4.857683991745159</v>
+        <v>5.396435320041327</v>
       </c>
       <c r="H16" t="n">
-        <v>2.204015424570608</v>
+        <v>2.323022884097642</v>
       </c>
       <c r="I16" t="n">
-        <v>29.58628114029827</v>
+        <v>34.36436563897902</v>
       </c>
       <c r="J16" t="n">
-        <v>5.439327269092959</v>
+        <v>5.86211272827289</v>
       </c>
       <c r="K16" t="n">
-        <v>0.5847675200842553</v>
+        <v>2.094464284029546</v>
       </c>
     </row>
     <row r="17">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1090,28 +1090,28 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.9913223490750589</v>
+        <v>0.9858865666226108</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9884297987667452</v>
+        <v>0.9811820888301477</v>
       </c>
       <c r="F17" t="n">
-        <v>9.723681120066061</v>
+        <v>10.81247518970051</v>
       </c>
       <c r="G17" t="n">
-        <v>4.330197234636165</v>
+        <v>5.419353069239344</v>
       </c>
       <c r="H17" t="n">
-        <v>2.080912596587412</v>
+        <v>2.327950400940566</v>
       </c>
       <c r="I17" t="n">
-        <v>26.03823636847859</v>
+        <v>35.42723913274293</v>
       </c>
       <c r="J17" t="n">
-        <v>5.102767520520467</v>
+        <v>5.952078555659605</v>
       </c>
       <c r="K17" t="n">
-        <v>0.9371691844462521</v>
+        <v>2.506906523463603</v>
       </c>
     </row>
     <row r="18">
@@ -1121,36 +1121,36 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>normalize: False/fit_intercept: True/alpha: 0.05</t>
+          <t>default</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.9847379562375832</v>
+        <v>0.9604634768935373</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9796506083167776</v>
+        <v>0.9472846358580497</v>
       </c>
       <c r="F18" t="n">
-        <v>8.342530716029216</v>
+        <v>18.00584804673306</v>
       </c>
       <c r="G18" t="n">
-        <v>5.350753575872083</v>
+        <v>8.429227032204874</v>
       </c>
       <c r="H18" t="n">
-        <v>2.313169595138256</v>
+        <v>2.903313113015004</v>
       </c>
       <c r="I18" t="n">
-        <v>32.97262886161938</v>
+        <v>99.24373617080612</v>
       </c>
       <c r="J18" t="n">
-        <v>5.742179800530404</v>
+        <v>9.962115045049726</v>
       </c>
       <c r="K18" t="n">
-        <v>1.327004320987311</v>
+        <v>2.057557845008537</v>
       </c>
     </row>
     <row r="19">
@@ -1160,7 +1160,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1168,28 +1168,28 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.9913080623967049</v>
+        <v>0.9859272148331321</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9884107498622732</v>
+        <v>0.981236286444176</v>
       </c>
       <c r="F19" t="n">
-        <v>9.730655344942974</v>
+        <v>10.82754213475699</v>
       </c>
       <c r="G19" t="n">
-        <v>4.327341162846548</v>
+        <v>5.419625058810348</v>
       </c>
       <c r="H19" t="n">
-        <v>2.080226228766128</v>
+        <v>2.328008818456311</v>
       </c>
       <c r="I19" t="n">
-        <v>26.08110510232365</v>
+        <v>35.3252048625585</v>
       </c>
       <c r="J19" t="n">
-        <v>5.106966330643237</v>
+        <v>5.943501061037888</v>
       </c>
       <c r="K19" t="n">
-        <v>0.9478701580016372</v>
+        <v>2.477894955344792</v>
       </c>
     </row>
     <row r="20">
@@ -1199,36 +1199,36 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>normalize: True/fit_intercept: True/criterion: bic</t>
+          <t>normalize: False/fit_intercept: True/criterion: bic</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.991398670092772</v>
+        <v>0.9855178157563241</v>
       </c>
       <c r="E20" t="n">
-        <v>0.988531560123696</v>
+        <v>0.9806904210084322</v>
       </c>
       <c r="F20" t="n">
-        <v>9.643600785171358</v>
+        <v>10.80788753395722</v>
       </c>
       <c r="G20" t="n">
-        <v>4.480742583891028</v>
+        <v>5.449274755842302</v>
       </c>
       <c r="H20" t="n">
-        <v>2.116776460538766</v>
+        <v>2.334368170585416</v>
       </c>
       <c r="I20" t="n">
-        <v>25.80922684547654</v>
+        <v>36.35286968421935</v>
       </c>
       <c r="J20" t="n">
-        <v>5.080278225203472</v>
+        <v>6.029334099568488</v>
       </c>
       <c r="K20" t="n">
-        <v>0.7753552184930907</v>
+        <v>2.669498630822106</v>
       </c>
     </row>
     <row r="21">
@@ -1238,7 +1238,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1246,28 +1246,28 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.9910718957713713</v>
+        <v>0.9862975178373594</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9880958610284951</v>
+        <v>0.9817300237831459</v>
       </c>
       <c r="F21" t="n">
-        <v>9.759519116259312</v>
+        <v>9.527663346272874</v>
       </c>
       <c r="G21" t="n">
-        <v>4.342011314858286</v>
+        <v>5.547959643245955</v>
       </c>
       <c r="H21" t="n">
-        <v>2.083749340697745</v>
+        <v>2.355410716466654</v>
       </c>
       <c r="I21" t="n">
-        <v>26.78974877397756</v>
+        <v>35.93420825773995</v>
       </c>
       <c r="J21" t="n">
-        <v>5.175881448987946</v>
+        <v>5.994514847570231</v>
       </c>
       <c r="K21" t="n">
-        <v>1.008249996397359</v>
+        <v>0.4012007676083682</v>
       </c>
     </row>
     <row r="22">
@@ -1277,36 +1277,36 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>loss: epsilon_insensitive/epsilon: 0.1/C: 50</t>
+          <t>loss: squared_epsilon_insensitive/epsilon: 0/C: 5</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.9926052158134857</v>
+        <v>0.98552249644859</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9901402877513142</v>
+        <v>0.9806966619314533</v>
       </c>
       <c r="F22" t="n">
-        <v>11.10888930239261</v>
+        <v>10.35094127830876</v>
       </c>
       <c r="G22" t="n">
-        <v>3.618779355937456</v>
+        <v>5.47579981558126</v>
       </c>
       <c r="H22" t="n">
-        <v>1.902308953860402</v>
+        <v>2.340042695247516</v>
       </c>
       <c r="I22" t="n">
-        <v>22.18885504934659</v>
+        <v>36.34112031042964</v>
       </c>
       <c r="J22" t="n">
-        <v>4.710504755262072</v>
+        <v>6.028359669962438</v>
       </c>
       <c r="K22" t="n">
-        <v>0.9172069493084416</v>
+        <v>2.797194473915273</v>
       </c>
     </row>
     <row r="23">
@@ -1316,36 +1316,36 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>nu: 1/kernel: rbf/gamma: 0.01/C: 20000</t>
+          <t>nu: 0.01/kernel: sigmoid/gamma: 0.0001/C: 100000</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.9974889163280239</v>
+        <v>0.1917950719520626</v>
       </c>
       <c r="E23" t="n">
-        <v>0.9966518884373653</v>
+        <v>-0.0776065707305833</v>
       </c>
       <c r="F23" t="n">
-        <v>6.820715624251761</v>
+        <v>68.05770179866666</v>
       </c>
       <c r="G23" t="n">
-        <v>1.61011479771774</v>
+        <v>35.75978546768628</v>
       </c>
       <c r="H23" t="n">
-        <v>1.268902989876586</v>
+        <v>5.979948617478772</v>
       </c>
       <c r="I23" t="n">
-        <v>5.281404555616716</v>
+        <v>2028.738754673741</v>
       </c>
       <c r="J23" t="n">
-        <v>2.298130665479384</v>
+        <v>45.04152256167348</v>
       </c>
       <c r="K23" t="n">
-        <v>0.7256677159812813</v>
+        <v>1.25712151558167</v>
       </c>
     </row>
     <row r="24">
@@ -1355,7 +1355,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1363,28 +1363,28 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.9602678170731903</v>
+        <v>0.9471168534958073</v>
       </c>
       <c r="E24" t="n">
-        <v>0.947023756097587</v>
+        <v>0.9294891379944098</v>
       </c>
       <c r="F24" t="n">
-        <v>15.92627632300401</v>
+        <v>20.1731404857955</v>
       </c>
       <c r="G24" t="n">
-        <v>10.22006214668353</v>
+        <v>10.18639173713235</v>
       </c>
       <c r="H24" t="n">
-        <v>3.196883192530427</v>
+        <v>3.191612717284532</v>
       </c>
       <c r="I24" t="n">
-        <v>119.1044277155055</v>
+        <v>132.7461452645105</v>
       </c>
       <c r="J24" t="n">
-        <v>10.91349750151185</v>
+        <v>11.5215513393167</v>
       </c>
       <c r="K24" t="n">
-        <v>1.847311514780583</v>
+        <v>3.343254092502247</v>
       </c>
     </row>
     <row r="25">
@@ -1394,7 +1394,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1402,28 +1402,28 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.9914818122615752</v>
+        <v>0.9861505789527807</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9886424163487669</v>
+        <v>0.9815341052703742</v>
       </c>
       <c r="F25" t="n">
-        <v>9.801220151983387</v>
+        <v>9.555304033238144</v>
       </c>
       <c r="G25" t="n">
-        <v>4.185374844115579</v>
+        <v>5.634958671136338</v>
       </c>
       <c r="H25" t="n">
-        <v>2.045818868843373</v>
+        <v>2.373806788922876</v>
       </c>
       <c r="I25" t="n">
-        <v>25.55974971598512</v>
+        <v>36.31954957159367</v>
       </c>
       <c r="J25" t="n">
-        <v>5.055665111138703</v>
+        <v>6.026570299232696</v>
       </c>
       <c r="K25" t="n">
-        <v>0.9846191733521503</v>
+        <v>0.408824060076549</v>
       </c>
     </row>
     <row r="26">
@@ -1433,7 +1433,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1441,28 +1441,28 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.9887352303207657</v>
+        <v>0.9852282362272531</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9849803070943542</v>
+        <v>0.9803043149696707</v>
       </c>
       <c r="F26" t="n">
-        <v>8.39744899494768</v>
+        <v>13.74633211974675</v>
       </c>
       <c r="G26" t="n">
-        <v>4.410660418958767</v>
+        <v>5.087720810867804</v>
       </c>
       <c r="H26" t="n">
-        <v>2.10015723672271</v>
+        <v>2.255597661567285</v>
       </c>
       <c r="I26" t="n">
-        <v>24.33678448489767</v>
+        <v>37.07976603537834</v>
       </c>
       <c r="J26" t="n">
-        <v>4.933232660730453</v>
+        <v>6.089315728009046</v>
       </c>
       <c r="K26" t="n">
-        <v>1.423224634336801</v>
+        <v>1.885423497576516</v>
       </c>
     </row>
     <row r="27">
@@ -1472,36 +1472,36 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>default</t>
+          <t>min_samples: 1/loss: absolute_loss</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.9910718957713713</v>
+        <v>0.9868373379031185</v>
       </c>
       <c r="E27" t="n">
-        <v>0.9880958610284951</v>
+        <v>0.9824497838708246</v>
       </c>
       <c r="F27" t="n">
-        <v>9.759519116259312</v>
+        <v>10.22669917735227</v>
       </c>
       <c r="G27" t="n">
-        <v>4.342011314858286</v>
+        <v>5.184240702942263</v>
       </c>
       <c r="H27" t="n">
-        <v>2.083749340697745</v>
+        <v>2.27689277370329</v>
       </c>
       <c r="I27" t="n">
-        <v>26.78974877397756</v>
+        <v>33.04063336401102</v>
       </c>
       <c r="J27" t="n">
-        <v>5.175881448987946</v>
+        <v>5.74809823889702</v>
       </c>
       <c r="K27" t="n">
-        <v>1.008249996397359</v>
+        <v>1.747650457449339</v>
       </c>
     </row>
     <row r="28">
@@ -1511,7 +1511,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1519,28 +1519,28 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.9991136864730743</v>
+        <v>0.9988428424442749</v>
       </c>
       <c r="E28" t="n">
-        <v>0.9988182486307657</v>
+        <v>0.9984571232590332</v>
       </c>
       <c r="F28" t="n">
-        <v>3.43984377999999</v>
+        <v>3.630354080000075</v>
       </c>
       <c r="G28" t="n">
-        <v>1.32211465647059</v>
+        <v>1.334194305882373</v>
       </c>
       <c r="H28" t="n">
-        <v>1.149832447128967</v>
+        <v>1.155073290264463</v>
       </c>
       <c r="I28" t="n">
-        <v>2.656885618277137</v>
+        <v>3.03459914057142</v>
       </c>
       <c r="J28" t="n">
-        <v>1.6299955884226</v>
+        <v>1.742010086242735</v>
       </c>
       <c r="K28" t="n">
-        <v>0.1178287700326892</v>
+        <v>0.1427371260241757</v>
       </c>
     </row>
     <row r="29">
@@ -1550,36 +1550,36 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>solver: sparse_cg/normalize: False/fit_intercept: True/alpha: 1</t>
+          <t>default</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.9913099760155636</v>
+        <v>0.9860761163890228</v>
       </c>
       <c r="E29" t="n">
-        <v>0.9884133013540848</v>
+        <v>0.9814348218520305</v>
       </c>
       <c r="F29" t="n">
-        <v>8.741948089975303</v>
+        <v>8.868482096518939</v>
       </c>
       <c r="G29" t="n">
-        <v>4.543947711653923</v>
+        <v>5.573437117941317</v>
       </c>
       <c r="H29" t="n">
-        <v>2.131653750413965</v>
+        <v>2.360812808746453</v>
       </c>
       <c r="I29" t="n">
-        <v>26.07536308059536</v>
+        <v>34.95143535610881</v>
       </c>
       <c r="J29" t="n">
-        <v>5.106404124292882</v>
+        <v>5.911973896771602</v>
       </c>
       <c r="K29" t="n">
-        <v>0.9602694725436502</v>
+        <v>2.72801337892266</v>
       </c>
     </row>
     <row r="30">
@@ -1589,36 +1589,36 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>default</t>
+          <t>normalize: False/gcv_mode: eigen/fit_intercept: True</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.9911598294556796</v>
+        <v>0.9855386902963195</v>
       </c>
       <c r="E30" t="n">
-        <v>0.9882131059409062</v>
+        <v>0.9807182537284259</v>
       </c>
       <c r="F30" t="n">
-        <v>9.598929065143437</v>
+        <v>10.36384665501048</v>
       </c>
       <c r="G30" t="n">
-        <v>4.349559810361415</v>
+        <v>5.47199638603862</v>
       </c>
       <c r="H30" t="n">
-        <v>2.085559831402929</v>
+        <v>2.339229870286077</v>
       </c>
       <c r="I30" t="n">
-        <v>26.52589418054258</v>
+        <v>36.30047085960842</v>
       </c>
       <c r="J30" t="n">
-        <v>5.150329521549333</v>
+        <v>6.02498720825268</v>
       </c>
       <c r="K30" t="n">
-        <v>1.002356451350274</v>
+        <v>2.793948536557211</v>
       </c>
     </row>
     <row r="31">
@@ -1628,7 +1628,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1636,28 +1636,28 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.9910908136591279</v>
+        <v>0.9862020246423787</v>
       </c>
       <c r="E31" t="n">
-        <v>0.9881210848788372</v>
+        <v>0.9816026995231716</v>
       </c>
       <c r="F31" t="n">
-        <v>9.681418375355378</v>
+        <v>9.651984400222851</v>
       </c>
       <c r="G31" t="n">
-        <v>4.358498404917627</v>
+        <v>5.561411716293115</v>
       </c>
       <c r="H31" t="n">
-        <v>2.087701704007933</v>
+        <v>2.358264556043939</v>
       </c>
       <c r="I31" t="n">
-        <v>26.73298359210311</v>
+        <v>36.18463532014376</v>
       </c>
       <c r="J31" t="n">
-        <v>5.170394916454942</v>
+        <v>6.015366598981625</v>
       </c>
       <c r="K31" t="n">
-        <v>1.000874387292069</v>
+        <v>0.4021119255477097</v>
       </c>
     </row>
     <row r="32">
@@ -1667,36 +1667,36 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>kernel: rbf/gamma: 0.01/epsilon: 0.01/C: 20000</t>
+          <t>kernel: sigmoid/gamma: 0.01/epsilon: 1.0/C: 5000</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.9984106694407948</v>
+        <v>0.9837955433770645</v>
       </c>
       <c r="E32" t="n">
-        <v>0.9978808925877264</v>
+        <v>0.978394057836086</v>
       </c>
       <c r="F32" t="n">
-        <v>5.280515757549572</v>
+        <v>10.5882702982145</v>
       </c>
       <c r="G32" t="n">
-        <v>1.500207276035427</v>
+        <v>5.523941464245285</v>
       </c>
       <c r="H32" t="n">
-        <v>1.224829488555622</v>
+        <v>2.350306674509794</v>
       </c>
       <c r="I32" t="n">
-        <v>4.768959379235794</v>
+        <v>42.49553563219968</v>
       </c>
       <c r="J32" t="n">
-        <v>2.183794720031119</v>
+        <v>6.51885999483036</v>
       </c>
       <c r="K32" t="n">
-        <v>0.4064659178720975</v>
+        <v>0.4787901291670473</v>
       </c>
     </row>
     <row r="33">
@@ -1706,36 +1706,36 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>default</t>
+          <t>learning_rate: 0.05/booster: gbtree</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.9992133829277974</v>
+        <v>0.9987470923905283</v>
       </c>
       <c r="E33" t="n">
-        <v>0.9989511772370632</v>
+        <v>0.9983294565207044</v>
       </c>
       <c r="F33" t="n">
-        <v>3.195059539306641</v>
+        <v>3.628339296630859</v>
       </c>
       <c r="G33" t="n">
-        <v>1.018061412395</v>
+        <v>1.307016884193981</v>
       </c>
       <c r="H33" t="n">
-        <v>1.008990293508813</v>
+        <v>1.143248391292977</v>
       </c>
       <c r="I33" t="n">
-        <v>1.699433783686425</v>
+        <v>3.28569980475623</v>
       </c>
       <c r="J33" t="n">
-        <v>1.303623328913082</v>
+        <v>1.812649939937723</v>
       </c>
       <c r="K33" t="n">
-        <v>0.1654659813424175</v>
+        <v>0.08495895651026102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[NEW] Save models feature
</commit_message>
<xml_diff>
--- a/examples/regression/skl_regressor_test_summary.xlsx
+++ b/examples/regression/skl_regressor_test_summary.xlsx
@@ -501,32 +501,32 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>n_estimators: 50/loss: exponential/learning_rate: 0.3</t>
+          <t>n_estimators: 1000/loss: linear/learning_rate: 0.05</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.9968105280705966</v>
+        <v>0.9970740986212113</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9957473707607954</v>
+        <v>0.9960987981616151</v>
       </c>
       <c r="F2" t="n">
-        <v>6.109256117647064</v>
+        <v>5.951542888888881</v>
       </c>
       <c r="G2" t="n">
-        <v>2.488673687089965</v>
+        <v>2.357949350763127</v>
       </c>
       <c r="H2" t="n">
-        <v>1.577553069500347</v>
+        <v>1.53556157504775</v>
       </c>
       <c r="I2" t="n">
-        <v>8.364261831033858</v>
+        <v>7.673058664776945</v>
       </c>
       <c r="J2" t="n">
-        <v>2.892103357598732</v>
+        <v>2.770028639703378</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2155627060651892</v>
+        <v>0.2066480472838494</v>
       </c>
     </row>
     <row r="3">
@@ -544,28 +544,28 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.9988560555848621</v>
+        <v>0.9989312542656047</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9984747407798161</v>
+        <v>0.9985750056874729</v>
       </c>
       <c r="F3" t="n">
-        <v>3.425956200000073</v>
+        <v>3.63680051</v>
       </c>
       <c r="G3" t="n">
-        <v>1.322533833529427</v>
+        <v>1.230832914117661</v>
       </c>
       <c r="H3" t="n">
-        <v>1.150014710136104</v>
+        <v>1.109429093776462</v>
       </c>
       <c r="I3" t="n">
-        <v>2.999948210910336</v>
+        <v>2.802742695702421</v>
       </c>
       <c r="J3" t="n">
-        <v>1.732035857281926</v>
+        <v>1.674139389567793</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1316424817931592</v>
+        <v>0.1481169740771154</v>
       </c>
     </row>
     <row r="4">
@@ -622,28 +622,28 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.9979738033433034</v>
+        <v>0.9983952421432284</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9972984044577379</v>
+        <v>0.9978603228576378</v>
       </c>
       <c r="F5" t="n">
         <v>4.138573999999991</v>
       </c>
       <c r="G5" t="n">
-        <v>1.993801235294116</v>
+        <v>1.639556411764704</v>
       </c>
       <c r="H5" t="n">
-        <v>1.412020267309969</v>
+        <v>1.280451643665119</v>
       </c>
       <c r="I5" t="n">
-        <v>5.313619223777232</v>
+        <v>4.208412924316758</v>
       </c>
       <c r="J5" t="n">
-        <v>2.305128895263176</v>
+        <v>2.051441669732961</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1371398890472471</v>
+        <v>0.131964946538029</v>
       </c>
     </row>
     <row r="6">
@@ -778,28 +778,28 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.9986523022906715</v>
+        <v>0.9989569740841011</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9982030697208953</v>
+        <v>0.9986092987788014</v>
       </c>
       <c r="F9" t="n">
-        <v>4.138573999999991</v>
+        <v>3.222245999999998</v>
       </c>
       <c r="G9" t="n">
-        <v>1.411778411764706</v>
+        <v>1.312411411764706</v>
       </c>
       <c r="H9" t="n">
-        <v>1.188182819167449</v>
+        <v>1.145605260010928</v>
       </c>
       <c r="I9" t="n">
-        <v>3.534283028481468</v>
+        <v>2.735293506334235</v>
       </c>
       <c r="J9" t="n">
-        <v>1.879968890296185</v>
+        <v>1.653872276306195</v>
       </c>
       <c r="K9" t="n">
-        <v>0.04215737014596937</v>
+        <v>0.1251400952923244</v>
       </c>
     </row>
     <row r="10">
@@ -817,28 +817,28 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.9992304978263927</v>
+        <v>0.9992519435987042</v>
       </c>
       <c r="E10" t="n">
-        <v>0.998973997101857</v>
+        <v>0.9990025914649389</v>
       </c>
       <c r="F10" t="n">
-        <v>2.795443600000084</v>
+        <v>2.941553650000102</v>
       </c>
       <c r="G10" t="n">
-        <v>1.158941678823537</v>
+        <v>1.108323341764711</v>
       </c>
       <c r="H10" t="n">
-        <v>1.076541536041939</v>
+        <v>1.052769367793683</v>
       </c>
       <c r="I10" t="n">
-        <v>2.017988495294463</v>
+        <v>1.961747820113202</v>
       </c>
       <c r="J10" t="n">
-        <v>1.420559219214202</v>
+        <v>1.400624082369428</v>
       </c>
       <c r="K10" t="n">
-        <v>0.06739951589098545</v>
+        <v>0.06854339489521746</v>
       </c>
     </row>
     <row r="11">
@@ -862,22 +862,22 @@
         <v>0.9985851133096624</v>
       </c>
       <c r="F11" t="n">
-        <v>5.394667161180289</v>
+        <v>5.394667161180282</v>
       </c>
       <c r="G11" t="n">
-        <v>1.132850583870979</v>
+        <v>1.132850583870978</v>
       </c>
       <c r="H11" t="n">
-        <v>1.064354538615296</v>
+        <v>1.064354538615295</v>
       </c>
       <c r="I11" t="n">
-        <v>2.782862571260226</v>
+        <v>2.782862571260219</v>
       </c>
       <c r="J11" t="n">
-        <v>1.668191407261237</v>
+        <v>1.668191407261235</v>
       </c>
       <c r="K11" t="n">
-        <v>0.2001410298244644</v>
+        <v>0.2001410298244641</v>
       </c>
     </row>
     <row r="12">
@@ -1285,28 +1285,28 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.98552249644859</v>
+        <v>0.9855166402880439</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9806966619314533</v>
+        <v>0.9806888537173918</v>
       </c>
       <c r="F22" t="n">
-        <v>10.35094127830876</v>
+        <v>10.35501331098474</v>
       </c>
       <c r="G22" t="n">
-        <v>5.47579981558126</v>
+        <v>5.476754993133656</v>
       </c>
       <c r="H22" t="n">
-        <v>2.340042695247516</v>
+        <v>2.340246780391687</v>
       </c>
       <c r="I22" t="n">
-        <v>36.34112031042964</v>
+        <v>36.35582031959951</v>
       </c>
       <c r="J22" t="n">
-        <v>6.028359669962438</v>
+        <v>6.029578784591799</v>
       </c>
       <c r="K22" t="n">
-        <v>2.797194473915273</v>
+        <v>2.79757483068511</v>
       </c>
     </row>
     <row r="23">
@@ -1441,28 +1441,28 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.9852282362272531</v>
+        <v>0.9813950768443573</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9803043149696707</v>
+        <v>0.9751934357924764</v>
       </c>
       <c r="F26" t="n">
-        <v>13.74633211974675</v>
+        <v>10.12644693781989</v>
       </c>
       <c r="G26" t="n">
-        <v>5.087720810867804</v>
+        <v>5.890605791584575</v>
       </c>
       <c r="H26" t="n">
-        <v>2.255597661567285</v>
+        <v>2.427057022730322</v>
       </c>
       <c r="I26" t="n">
-        <v>37.07976603537834</v>
+        <v>46.70168087782371</v>
       </c>
       <c r="J26" t="n">
-        <v>6.089315728009046</v>
+        <v>6.833862807945716</v>
       </c>
       <c r="K26" t="n">
-        <v>1.885423497576516</v>
+        <v>3.344861601269455</v>
       </c>
     </row>
     <row r="27">
@@ -1480,28 +1480,28 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.9868373379031185</v>
+        <v>0.987108096335833</v>
       </c>
       <c r="E27" t="n">
-        <v>0.9824497838708246</v>
+        <v>0.9828107951144439</v>
       </c>
       <c r="F27" t="n">
-        <v>10.22669917735227</v>
+        <v>11.59310318431117</v>
       </c>
       <c r="G27" t="n">
-        <v>5.184240702942263</v>
+        <v>4.589529243119732</v>
       </c>
       <c r="H27" t="n">
-        <v>2.27689277370329</v>
+        <v>2.142318660498417</v>
       </c>
       <c r="I27" t="n">
-        <v>33.04063336401102</v>
+        <v>32.36098132708345</v>
       </c>
       <c r="J27" t="n">
-        <v>5.74809823889702</v>
+        <v>5.688671314734527</v>
       </c>
       <c r="K27" t="n">
-        <v>1.747650457449339</v>
+        <v>1.524179323399373</v>
       </c>
     </row>
     <row r="28">
@@ -1519,28 +1519,28 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.9988428424442749</v>
+        <v>0.9988970412247323</v>
       </c>
       <c r="E28" t="n">
-        <v>0.9984571232590332</v>
+        <v>0.9985293882996431</v>
       </c>
       <c r="F28" t="n">
-        <v>3.630354080000075</v>
+        <v>3.447691430000091</v>
       </c>
       <c r="G28" t="n">
-        <v>1.334194305882373</v>
+        <v>1.301806200588247</v>
       </c>
       <c r="H28" t="n">
-        <v>1.155073290264463</v>
+        <v>1.140967221522269</v>
       </c>
       <c r="I28" t="n">
-        <v>3.03459914057142</v>
+        <v>2.892465019092028</v>
       </c>
       <c r="J28" t="n">
-        <v>1.742010086242735</v>
+        <v>1.700724851083216</v>
       </c>
       <c r="K28" t="n">
-        <v>0.1427371260241757</v>
+        <v>0.1242185294832174</v>
       </c>
     </row>
     <row r="29">
@@ -1636,28 +1636,28 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.9862020246423787</v>
+        <v>0.9861638074326824</v>
       </c>
       <c r="E31" t="n">
-        <v>0.9816026995231716</v>
+        <v>0.9815517432435765</v>
       </c>
       <c r="F31" t="n">
-        <v>9.651984400222851</v>
+        <v>9.712292007094582</v>
       </c>
       <c r="G31" t="n">
-        <v>5.561411716293115</v>
+        <v>5.56719217776397</v>
       </c>
       <c r="H31" t="n">
-        <v>2.358264556043939</v>
+        <v>2.359489813023987</v>
       </c>
       <c r="I31" t="n">
-        <v>36.18463532014376</v>
+        <v>36.28485841519763</v>
       </c>
       <c r="J31" t="n">
-        <v>6.015366598981625</v>
+        <v>6.023691427621242</v>
       </c>
       <c r="K31" t="n">
-        <v>0.4021119255477097</v>
+        <v>0.4025348537241473</v>
       </c>
     </row>
     <row r="32">

</xml_diff>